<commit_message>
Draft 29 Oct 6pm
Changed Register File to switch statements
Added 1 more function into memory.cpp
Settled the main.cpp
Didnt really do anything for instructions.cpp so skip that
Simulator.cpp:
1. added new functions
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\C++\MipsSim\mjnwlc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{5F3E25F7-58A4-4BB2-AC71-7B38F82107A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF0FF93-2CA2-41A3-BB3F-CFC8AEED7564}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-852" yWindow="540" windowWidth="23280" windowHeight="12000" xr2:uid="{DE50BC15-ADE5-4BB9-9D10-6F39E6D74606}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DE50BC15-ADE5-4BB9-9D10-6F39E6D74606}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="126">
   <si>
     <t>Code</t>
   </si>
@@ -406,6 +406,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -827,23 +830,23 @@
   <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -854,7 +857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -868,7 +871,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -882,7 +885,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -896,7 +899,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -910,7 +913,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -924,7 +927,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -938,7 +941,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -952,7 +955,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
@@ -966,7 +969,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -980,7 +983,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
@@ -994,7 +997,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
@@ -1008,7 +1011,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>29</v>
       </c>
@@ -1022,7 +1025,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>31</v>
       </c>
@@ -1036,7 +1039,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>33</v>
       </c>
@@ -1050,7 +1053,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>35</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
@@ -1078,7 +1081,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>39</v>
       </c>
@@ -1092,7 +1095,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>41</v>
       </c>
@@ -1106,7 +1109,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>43</v>
       </c>
@@ -1120,7 +1123,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>45</v>
       </c>
@@ -1134,7 +1137,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>47</v>
       </c>
@@ -1148,7 +1151,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>49</v>
       </c>
@@ -1162,7 +1165,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>51</v>
       </c>
@@ -1176,7 +1179,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>53</v>
       </c>
@@ -1190,7 +1193,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>55</v>
       </c>
@@ -1204,7 +1207,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>57</v>
       </c>
@@ -1218,7 +1221,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>59</v>
       </c>
@@ -1232,7 +1235,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>62</v>
       </c>
@@ -1246,7 +1249,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>64</v>
       </c>
@@ -1260,7 +1263,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>66</v>
       </c>
@@ -1274,7 +1277,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>68</v>
       </c>
@@ -1288,7 +1291,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>70</v>
       </c>
@@ -1302,7 +1305,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>72</v>
       </c>
@@ -1316,7 +1319,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>74</v>
       </c>
@@ -1330,7 +1333,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>76</v>
       </c>
@@ -1344,7 +1347,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>78</v>
       </c>
@@ -1358,7 +1361,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>80</v>
       </c>
@@ -1372,7 +1375,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>82</v>
       </c>
@@ -1386,7 +1389,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>84</v>
       </c>
@@ -1400,7 +1403,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>86</v>
       </c>
@@ -1414,7 +1417,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>88</v>
       </c>
@@ -1428,7 +1431,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>90</v>
       </c>
@@ -1442,7 +1445,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>92</v>
       </c>
@@ -1456,7 +1459,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>94</v>
       </c>
@@ -1470,7 +1473,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>96</v>
       </c>
@@ -1484,7 +1487,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>98</v>
       </c>
@@ -1498,7 +1501,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>99</v>
       </c>
@@ -1512,7 +1515,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>101</v>
       </c>
@@ -1526,7 +1529,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>103</v>
       </c>
@@ -1540,7 +1543,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>105</v>
       </c>
@@ -1554,7 +1557,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>107</v>
       </c>
@@ -1568,7 +1571,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>109</v>
       </c>
@@ -1582,7 +1585,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>111</v>
       </c>
@@ -1596,7 +1599,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>113</v>
       </c>
@@ -1607,7 +1610,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>116</v>
       </c>
@@ -1616,7 +1619,7 @@
       </c>
       <c r="C57" s="4"/>
     </row>
-    <row r="58" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>118</v>
       </c>
@@ -1625,7 +1628,7 @@
       </c>
       <c r="C58" s="5"/>
     </row>
-    <row r="59" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>120</v>
       </c>
@@ -1633,6 +1636,9 @@
         <v>121</v>
       </c>
       <c r="C59" s="1"/>
+      <c r="D59" s="2" t="s">
+        <v>125</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>